<commit_message>
visu good model only
</commit_message>
<xml_diff>
--- a/Results/xlsx/planning_toy_instance.xlsx
+++ b/Results/xlsx/planning_toy_instance.xlsx
@@ -534,13 +534,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -552,16 +552,16 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -584,37 +584,37 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -623,10 +623,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -637,37 +637,37 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -687,25 +687,25 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -717,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -729,10 +729,10 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -740,16 +740,16 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -758,22 +758,22 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -782,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -846,7 +846,7 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -855,16 +855,16 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -899,16 +899,16 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -952,25 +952,25 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1005,10 +1005,10 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1100,10 +1100,10 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1241,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1276,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -1341,22 +1341,22 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1365,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>